<commit_message>
Updated experiment description with metadata
</commit_message>
<xml_diff>
--- a/data/flaviolin/DBTL0/experiment_description.xlsx
+++ b/data/flaviolin/DBTL0/experiment_description.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,10 +461,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Shaking speed[rpm]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Growth Temperature</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Humidity[%]</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Plate</t>
         </is>
@@ -493,9 +503,15 @@
         <v>1500</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
-      </c>
-      <c r="G2" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G2" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2" t="n">
+        <v>90</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -524,9 +540,15 @@
         <v>1500</v>
       </c>
       <c r="F3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G3" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G3" t="n">
+        <v>30</v>
+      </c>
+      <c r="H3" t="n">
+        <v>90</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -555,9 +577,15 @@
         <v>1500</v>
       </c>
       <c r="F4" t="n">
-        <v>30</v>
-      </c>
-      <c r="G4" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30</v>
+      </c>
+      <c r="H4" t="n">
+        <v>90</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -586,9 +614,15 @@
         <v>1500</v>
       </c>
       <c r="F5" t="n">
-        <v>30</v>
-      </c>
-      <c r="G5" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G5" t="n">
+        <v>30</v>
+      </c>
+      <c r="H5" t="n">
+        <v>90</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -617,9 +651,15 @@
         <v>1500</v>
       </c>
       <c r="F6" t="n">
-        <v>30</v>
-      </c>
-      <c r="G6" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G6" t="n">
+        <v>30</v>
+      </c>
+      <c r="H6" t="n">
+        <v>90</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -648,9 +688,15 @@
         <v>1500</v>
       </c>
       <c r="F7" t="n">
-        <v>30</v>
-      </c>
-      <c r="G7" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G7" t="n">
+        <v>30</v>
+      </c>
+      <c r="H7" t="n">
+        <v>90</v>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -679,9 +725,15 @@
         <v>1500</v>
       </c>
       <c r="F8" t="n">
-        <v>30</v>
-      </c>
-      <c r="G8" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G8" t="n">
+        <v>30</v>
+      </c>
+      <c r="H8" t="n">
+        <v>90</v>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -710,9 +762,15 @@
         <v>1500</v>
       </c>
       <c r="F9" t="n">
-        <v>30</v>
-      </c>
-      <c r="G9" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G9" t="n">
+        <v>30</v>
+      </c>
+      <c r="H9" t="n">
+        <v>90</v>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -741,9 +799,15 @@
         <v>1500</v>
       </c>
       <c r="F10" t="n">
-        <v>30</v>
-      </c>
-      <c r="G10" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G10" t="n">
+        <v>30</v>
+      </c>
+      <c r="H10" t="n">
+        <v>90</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -772,9 +836,15 @@
         <v>1500</v>
       </c>
       <c r="F11" t="n">
-        <v>30</v>
-      </c>
-      <c r="G11" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G11" t="n">
+        <v>30</v>
+      </c>
+      <c r="H11" t="n">
+        <v>90</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -803,9 +873,15 @@
         <v>1500</v>
       </c>
       <c r="F12" t="n">
-        <v>30</v>
-      </c>
-      <c r="G12" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G12" t="n">
+        <v>30</v>
+      </c>
+      <c r="H12" t="n">
+        <v>90</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -834,9 +910,15 @@
         <v>1500</v>
       </c>
       <c r="F13" t="n">
-        <v>30</v>
-      </c>
-      <c r="G13" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G13" t="n">
+        <v>30</v>
+      </c>
+      <c r="H13" t="n">
+        <v>90</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -865,9 +947,15 @@
         <v>1500</v>
       </c>
       <c r="F14" t="n">
-        <v>30</v>
-      </c>
-      <c r="G14" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G14" t="n">
+        <v>30</v>
+      </c>
+      <c r="H14" t="n">
+        <v>90</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -896,9 +984,15 @@
         <v>1500</v>
       </c>
       <c r="F15" t="n">
-        <v>30</v>
-      </c>
-      <c r="G15" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G15" t="n">
+        <v>30</v>
+      </c>
+      <c r="H15" t="n">
+        <v>90</v>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -927,9 +1021,15 @@
         <v>1500</v>
       </c>
       <c r="F16" t="n">
-        <v>30</v>
-      </c>
-      <c r="G16" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G16" t="n">
+        <v>30</v>
+      </c>
+      <c r="H16" t="n">
+        <v>90</v>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -958,9 +1058,15 @@
         <v>1500</v>
       </c>
       <c r="F17" t="n">
-        <v>30</v>
-      </c>
-      <c r="G17" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G17" t="n">
+        <v>30</v>
+      </c>
+      <c r="H17" t="n">
+        <v>90</v>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -989,9 +1095,15 @@
         <v>1500</v>
       </c>
       <c r="F18" t="n">
-        <v>30</v>
-      </c>
-      <c r="G18" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G18" t="n">
+        <v>30</v>
+      </c>
+      <c r="H18" t="n">
+        <v>90</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1020,9 +1132,15 @@
         <v>1500</v>
       </c>
       <c r="F19" t="n">
-        <v>30</v>
-      </c>
-      <c r="G19" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G19" t="n">
+        <v>30</v>
+      </c>
+      <c r="H19" t="n">
+        <v>90</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1051,9 +1169,15 @@
         <v>1500</v>
       </c>
       <c r="F20" t="n">
-        <v>30</v>
-      </c>
-      <c r="G20" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G20" t="n">
+        <v>30</v>
+      </c>
+      <c r="H20" t="n">
+        <v>90</v>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1082,9 +1206,15 @@
         <v>1500</v>
       </c>
       <c r="F21" t="n">
-        <v>30</v>
-      </c>
-      <c r="G21" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G21" t="n">
+        <v>30</v>
+      </c>
+      <c r="H21" t="n">
+        <v>90</v>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1113,9 +1243,15 @@
         <v>1500</v>
       </c>
       <c r="F22" t="n">
-        <v>30</v>
-      </c>
-      <c r="G22" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G22" t="n">
+        <v>30</v>
+      </c>
+      <c r="H22" t="n">
+        <v>90</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1144,9 +1280,15 @@
         <v>1500</v>
       </c>
       <c r="F23" t="n">
-        <v>30</v>
-      </c>
-      <c r="G23" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G23" t="n">
+        <v>30</v>
+      </c>
+      <c r="H23" t="n">
+        <v>90</v>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1175,9 +1317,15 @@
         <v>1500</v>
       </c>
       <c r="F24" t="n">
-        <v>30</v>
-      </c>
-      <c r="G24" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G24" t="n">
+        <v>30</v>
+      </c>
+      <c r="H24" t="n">
+        <v>90</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1206,9 +1354,15 @@
         <v>1500</v>
       </c>
       <c r="F25" t="n">
-        <v>30</v>
-      </c>
-      <c r="G25" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G25" t="n">
+        <v>30</v>
+      </c>
+      <c r="H25" t="n">
+        <v>90</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1237,9 +1391,15 @@
         <v>1500</v>
       </c>
       <c r="F26" t="n">
-        <v>30</v>
-      </c>
-      <c r="G26" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G26" t="n">
+        <v>30</v>
+      </c>
+      <c r="H26" t="n">
+        <v>90</v>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1268,9 +1428,15 @@
         <v>1500</v>
       </c>
       <c r="F27" t="n">
-        <v>30</v>
-      </c>
-      <c r="G27" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G27" t="n">
+        <v>30</v>
+      </c>
+      <c r="H27" t="n">
+        <v>90</v>
+      </c>
+      <c r="I27" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1299,9 +1465,15 @@
         <v>1500</v>
       </c>
       <c r="F28" t="n">
-        <v>30</v>
-      </c>
-      <c r="G28" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G28" t="n">
+        <v>30</v>
+      </c>
+      <c r="H28" t="n">
+        <v>90</v>
+      </c>
+      <c r="I28" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1330,9 +1502,15 @@
         <v>1500</v>
       </c>
       <c r="F29" t="n">
-        <v>30</v>
-      </c>
-      <c r="G29" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G29" t="n">
+        <v>30</v>
+      </c>
+      <c r="H29" t="n">
+        <v>90</v>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1361,9 +1539,15 @@
         <v>1500</v>
       </c>
       <c r="F30" t="n">
-        <v>30</v>
-      </c>
-      <c r="G30" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G30" t="n">
+        <v>30</v>
+      </c>
+      <c r="H30" t="n">
+        <v>90</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1392,9 +1576,15 @@
         <v>1500</v>
       </c>
       <c r="F31" t="n">
-        <v>30</v>
-      </c>
-      <c r="G31" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G31" t="n">
+        <v>30</v>
+      </c>
+      <c r="H31" t="n">
+        <v>90</v>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1423,9 +1613,15 @@
         <v>1500</v>
       </c>
       <c r="F32" t="n">
-        <v>30</v>
-      </c>
-      <c r="G32" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G32" t="n">
+        <v>30</v>
+      </c>
+      <c r="H32" t="n">
+        <v>90</v>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1454,9 +1650,15 @@
         <v>1500</v>
       </c>
       <c r="F33" t="n">
-        <v>30</v>
-      </c>
-      <c r="G33" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G33" t="n">
+        <v>30</v>
+      </c>
+      <c r="H33" t="n">
+        <v>90</v>
+      </c>
+      <c r="I33" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1485,9 +1687,15 @@
         <v>1500</v>
       </c>
       <c r="F34" t="n">
-        <v>30</v>
-      </c>
-      <c r="G34" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G34" t="n">
+        <v>30</v>
+      </c>
+      <c r="H34" t="n">
+        <v>90</v>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1516,9 +1724,15 @@
         <v>1500</v>
       </c>
       <c r="F35" t="n">
-        <v>30</v>
-      </c>
-      <c r="G35" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G35" t="n">
+        <v>30</v>
+      </c>
+      <c r="H35" t="n">
+        <v>90</v>
+      </c>
+      <c r="I35" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1547,9 +1761,15 @@
         <v>1500</v>
       </c>
       <c r="F36" t="n">
-        <v>30</v>
-      </c>
-      <c r="G36" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G36" t="n">
+        <v>30</v>
+      </c>
+      <c r="H36" t="n">
+        <v>90</v>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1578,9 +1798,15 @@
         <v>1500</v>
       </c>
       <c r="F37" t="n">
-        <v>30</v>
-      </c>
-      <c r="G37" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G37" t="n">
+        <v>30</v>
+      </c>
+      <c r="H37" t="n">
+        <v>90</v>
+      </c>
+      <c r="I37" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1609,9 +1835,15 @@
         <v>1500</v>
       </c>
       <c r="F38" t="n">
-        <v>30</v>
-      </c>
-      <c r="G38" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G38" t="n">
+        <v>30</v>
+      </c>
+      <c r="H38" t="n">
+        <v>90</v>
+      </c>
+      <c r="I38" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1640,9 +1872,15 @@
         <v>1500</v>
       </c>
       <c r="F39" t="n">
-        <v>30</v>
-      </c>
-      <c r="G39" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G39" t="n">
+        <v>30</v>
+      </c>
+      <c r="H39" t="n">
+        <v>90</v>
+      </c>
+      <c r="I39" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1671,9 +1909,15 @@
         <v>1500</v>
       </c>
       <c r="F40" t="n">
-        <v>30</v>
-      </c>
-      <c r="G40" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G40" t="n">
+        <v>30</v>
+      </c>
+      <c r="H40" t="n">
+        <v>90</v>
+      </c>
+      <c r="I40" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1702,9 +1946,15 @@
         <v>1500</v>
       </c>
       <c r="F41" t="n">
-        <v>30</v>
-      </c>
-      <c r="G41" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G41" t="n">
+        <v>30</v>
+      </c>
+      <c r="H41" t="n">
+        <v>90</v>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1733,9 +1983,15 @@
         <v>1500</v>
       </c>
       <c r="F42" t="n">
-        <v>30</v>
-      </c>
-      <c r="G42" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G42" t="n">
+        <v>30</v>
+      </c>
+      <c r="H42" t="n">
+        <v>90</v>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1764,9 +2020,15 @@
         <v>1500</v>
       </c>
       <c r="F43" t="n">
-        <v>30</v>
-      </c>
-      <c r="G43" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G43" t="n">
+        <v>30</v>
+      </c>
+      <c r="H43" t="n">
+        <v>90</v>
+      </c>
+      <c r="I43" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1795,9 +2057,15 @@
         <v>1500</v>
       </c>
       <c r="F44" t="n">
-        <v>30</v>
-      </c>
-      <c r="G44" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G44" t="n">
+        <v>30</v>
+      </c>
+      <c r="H44" t="n">
+        <v>90</v>
+      </c>
+      <c r="I44" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1826,9 +2094,15 @@
         <v>1500</v>
       </c>
       <c r="F45" t="n">
-        <v>30</v>
-      </c>
-      <c r="G45" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G45" t="n">
+        <v>30</v>
+      </c>
+      <c r="H45" t="n">
+        <v>90</v>
+      </c>
+      <c r="I45" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1857,9 +2131,15 @@
         <v>1500</v>
       </c>
       <c r="F46" t="n">
-        <v>30</v>
-      </c>
-      <c r="G46" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G46" t="n">
+        <v>30</v>
+      </c>
+      <c r="H46" t="n">
+        <v>90</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1888,9 +2168,15 @@
         <v>1500</v>
       </c>
       <c r="F47" t="n">
-        <v>30</v>
-      </c>
-      <c r="G47" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G47" t="n">
+        <v>30</v>
+      </c>
+      <c r="H47" t="n">
+        <v>90</v>
+      </c>
+      <c r="I47" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1919,9 +2205,15 @@
         <v>1500</v>
       </c>
       <c r="F48" t="n">
-        <v>30</v>
-      </c>
-      <c r="G48" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G48" t="n">
+        <v>30</v>
+      </c>
+      <c r="H48" t="n">
+        <v>90</v>
+      </c>
+      <c r="I48" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>
@@ -1950,9 +2242,15 @@
         <v>1500</v>
       </c>
       <c r="F49" t="n">
-        <v>30</v>
-      </c>
-      <c r="G49" t="inlineStr">
+        <v>800</v>
+      </c>
+      <c r="G49" t="n">
+        <v>30</v>
+      </c>
+      <c r="H49" t="n">
+        <v>90</v>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>m2p_flower</t>
         </is>

</xml_diff>